<commit_message>
Actualizacion de archivo match
</commit_message>
<xml_diff>
--- a/match.xlsx
+++ b/match.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Página1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Página1!$A$1:$Z$981</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Página1!$A$1:$Z$1026</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1518" uniqueCount="844">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1653" uniqueCount="963">
   <si>
     <t>Descripcion</t>
   </si>
@@ -44,7 +44,7 @@
     <t>CARGA DE GAS REFRIGERANTE POR LITRO PARA A.A TIPO SPLIT DE 12.000 BTU MARCA: RBD- TOKYO, MIDEA, VCP, CHUNLAN, GOTZE, MATSUI, SPRINGER, MIDAS, CONSUL, CARRIER</t>
   </si>
   <si>
-    <t>Manifold de manometros; Bomba de vacio; Balanza de refrigerante; Detector de fugas; Llave Allen/servicio; Termometro pinza</t>
+    <t>Manifold de manómetros; Bomba de vacio; Balanza de refrigerante; Detector de fugas; Llave Allen/servicio; Termómetro pinza</t>
   </si>
   <si>
     <t>Refrigerante (R22/R410/R407 segun equipo); Valvula Schrader; Cinta teflon; Nucleo Schrader; Tapas de valvula; Sellador de roscas</t>
@@ -62,7 +62,7 @@
     <t>SOLDADURA POR PERDIDA DE GAS A.A TIPO SPLIT DE 12.000 BTU MARCA: RBD- TOKYO, MIDEA, VCP, CHUNLAN, GOTZE, MATSUI, SPRINGER, MIDAS, CONSUL, CARRIER</t>
   </si>
   <si>
-    <t>Cortatubos; Soplete (MAP/oxi); Regulador y manometro de nitrogeno; Manifold de manometros; Detector de fugas; Abocardador/expansor</t>
+    <t>Cortatubos; Soplete (MAP/oxi); Regulador y manómetro de nitrogeno; Manifold de manómetros; Detector de fugas; Abocardador/expansor</t>
   </si>
   <si>
     <t>Varilla de soldadura (plata/fosforo); Nitrogeno; Refrigerante (segun equipo); Cinta teflon; Filtro secador; Pasta decapante; Lija/emery</t>
@@ -71,7 +71,7 @@
     <t>REBOBINADO DEL MOTOR VENTILADOR A.A TIPO SPLIT DE 12.000 BTU MARCA: RBD- TOKYO, MIDEA, VCP, CHUNLAN, GOTZE, MATSUI, SPRINGER, MIDAS, CONSUL, CARRIER</t>
   </si>
   <si>
-    <t>Banco/Herramientas de bobinado; Multimetro; Megger; Extractor de ruleman; Herramientas de mano</t>
+    <t>Banco/Herramientas de bobinado; Multímetro; Megger; Extractor de ruleman; Herramientas de mano</t>
   </si>
   <si>
     <t>Alambre de cobre esmaltado; Barniz aislante; Cinta aislante clase F/H; Termocontraible; Terminales tubulares; Cintillos; Ruleman (si aplica)</t>
@@ -89,7 +89,7 @@
     <t>CAMBIO DE CAPACITOR A.A TIPO SPLIT DE 12.000 BTU MARCA: RBD- TOKYO, MIDEA, VCP, CHUNLAN, GOTZE, MATSUI, SPRINGER, MIDAS, CONSUL, CARRIER</t>
   </si>
   <si>
-    <t>Destornilladores; Multimetro; Pinza amperimetrica; Alicate; Herramientas de mano</t>
+    <t>Destornilladores; Multímetro; Pinza amperimétrica; Alicate; Herramientas de mano</t>
   </si>
   <si>
     <t>Capacitor (uF y VAC segun placa); Terminales faston; Terminales tubulares; Cinta aisladora; Termocontraible; Cintillos</t>
@@ -98,7 +98,7 @@
     <t>CAMBIO DE TERMOSTATO A.A TIPO SPLIT DE 12.000 BTU MARCA: RBD- TOKYO, MIDEA, VCP, CHUNLAN, GOTZE, MATSUI, SPRINGER, MIDAS, CONSUL, CARRIER</t>
   </si>
   <si>
-    <t>Destornilladores; Multimetro; Alicate; Herramientas de mano</t>
+    <t>Destornilladores; Multímetro; Alicate; Herramientas de mano</t>
   </si>
   <si>
     <t>Termostato/sensor (segun equipo); Terminales tubular/horquilla; Cinta aisladora; Termocontraible; Cintillos; Conectores rapidos</t>
@@ -116,7 +116,7 @@
     <t>CAMBIO DE CONTACTOR A.A TIPO SPLIT DE 12.000 BTU MARCA: RBD- TOKYO, MIDEA, VCP, CHUNLAN, GOTZE, MATSUI, SPRINGER, MIDAS, CONSUL, CARRIER</t>
   </si>
   <si>
-    <t>Destornilladores; Multimetro; Pinza amperimetrica; Pelacables; Crimpadora</t>
+    <t>Destornilladores; Multímetro; Pinza amperimétrica; Pelacables; Crimpadora</t>
   </si>
   <si>
     <t>Contactor (amperaje segun equipo); Terminales horquilla; Terminales tubulares; Cinta aisladora; Termocontraible; Cintillos; Cable (si aplica)</t>
@@ -125,7 +125,7 @@
     <t>CAMBIO DE PLACA ELECTRONICA A.A TIPO SPLIT DE 12.000 BTU MARCA: RBD- TOKYO, MIDEA, VCP, CHUNLAN, GOTZE, MATSUI, SPRINGER, MIDAS, CONSUL, CARRIER</t>
   </si>
   <si>
-    <t>Destornilladores; Multimetro; Pinzas; Herramientas de mano</t>
+    <t>Destornilladores; Multímetro; Pinzas; Herramientas de mano</t>
   </si>
   <si>
     <t>Placa electronica (segun modelo); Conectores; Terminales tubulares; Cinta aisladora; Termocontraible; Cintillos</t>
@@ -134,7 +134,7 @@
     <t>TRASLADO DE EQUIPO A.A TIPO SPLIT DE 12.000 BTU MARCA: RBD- TOKYO, MIDEA, VCP, CHUNLAN, GOTZE, MATSUI, SPRINGER, MIDAS, CONSUL, CARRIER</t>
   </si>
   <si>
-    <t>Taladro; Nivel; Llaves; Manifold de manometros; Bomba de vacio; Cortatubos; Abocardador</t>
+    <t>Taladro; Nivel; Llaves; Manifold de manómetros; Bomba de vacio; Cortatubos; Abocardador</t>
   </si>
   <si>
     <t>Soportes metalicos; Tacos y tornillos; Tuberia de cobre; Aislacion termica; Cinta teflon; Cable electrico; Cintillos; Canaleta (si aplica)</t>
@@ -143,7 +143,7 @@
     <t>ARREGLO DE CABLEADO / CONEXION ELECTRICA A.A TIPO SPLIT DE 12.000 BTU MARCA: RBD- TOKYO, MIDEA, VCP, CHUNLAN, GOTZE, MATSUI, SPRINGER, MIDAS, CONSUL, CARRIER</t>
   </si>
   <si>
-    <t>Herramientas de mano; Multimetro; Pelacables; Crimpadora; Destornilladores</t>
+    <t>Herramientas de mano; Multímetro; Pelacables; Crimpadora; Destornilladores</t>
   </si>
   <si>
     <t>Terminales tubulares; Terminales horquilla; Terminales faston; Estaño; Flux; Cinta aisladora; Termocontraible; Cintillos; Conectores rapidos; Cable (segun seccion)</t>
@@ -185,7 +185,7 @@
     <t>CARGA DE GAS REFRIGERANTE POR LITRO PARA HELADERA MARCA: BRITANIA, ELECTROLUX, WHIRLPOOL, CONSUL, MABE, CONSUL, MABE, ELECTROLUX, WHIRLPOOL</t>
   </si>
   <si>
-    <t>Manifold de manometros; Balanza de refrigerante; Detector de fugas; Bomba de vacio (si aplica); Herramientas de mano</t>
+    <t>Manifold de manómetros; Balanza de refrigerante; Detector de fugas; Bomba de vacio (si aplica); Herramientas de mano</t>
   </si>
   <si>
     <t>Refrigerante (segun tipo); Valvula Schrader; Cinta teflon; Nucleo Schrader; Filtro secador; Sellador de roscas</t>
@@ -203,7 +203,7 @@
     <t>REBOBINADO DEL MOTOR VENTILADOR HELADERA MARCA: BRITANIA, ELECTROLUX, WHIRLPOOL, CONSUL, MABE, CONSUL, MABE, ELECTROLUX, WHIRLPOOL</t>
   </si>
   <si>
-    <t>Banco/Herramientas de bobinado; Multimetro; Megger; Herramientas de mano</t>
+    <t>Banco/Herramientas de bobinado; Multímetro; Megger; Herramientas de mano</t>
   </si>
   <si>
     <t>Alambre cobre esmaltado; Barniz aislante; Cinta aislante; Termocontraible; Terminales tubulares; Cintillos; Ruleman (si aplica)</t>
@@ -242,7 +242,7 @@
     <t>CAMBIO DE CONTACTOR HELADERA MARCA: BRITANIA, ELECTROLUX, WHIRLPOOL, CONSUL, MABE, CONSUL, MABE, ELECTROLUX, WHIRLPOOL</t>
   </si>
   <si>
-    <t>Destornilladores; Multimetro; Pelacables; Crimpadora; Herramientas de mano</t>
+    <t>Destornilladores; Multímetro; Pelacables; Crimpadora; Herramientas de mano</t>
   </si>
   <si>
     <t>Contactor/Relé (segun equipo); Terminales horquilla; Terminales tubulares; Estaño; Cinta aisladora; Termocontraible; Cintillos</t>
@@ -320,7 +320,7 @@
     <t>CAMBIO DE MOTOR COMPRESOR DE A.A TIPO SPLIT DE 24.000 BTU MAR..., SPRINGER, MIDAS, CONSUL, CARRIER, JAM, JAMES, CONFORT, STAR.</t>
   </si>
   <si>
-    <t>Bomba de vacio; Cortatubos; Manifold de manometros; Soplete; Multimetro</t>
+    <t>Bomba de vacio; Cortatubos; Manifold de manómetros; Soplete; Multímetro</t>
   </si>
   <si>
     <t>Compresor (segun modelo); Aceite de compresor; Filtro secador; Refrigerante (segun tipo); Cinta teflon; Terminales tubulares</t>
@@ -329,7 +329,7 @@
     <t>CAMBIO DE MOTOR VENTILADOR DE A.A TIPO SPLIT DE 24.000 BTU MA..., SPRINGER, MIDAS, CONSUL, CARRIER, JAM, JAMES, CONFORT, STAR.</t>
   </si>
   <si>
-    <t>Destornilladores; Multimetro; Pinza amperimetrica; Herramientas de mano</t>
+    <t>Destornilladores; Multímetro; Pinza amperimétrica; Herramientas de mano</t>
   </si>
   <si>
     <t>Motor ventilador (segun modelo); Capacitor (si aplica); Terminales faston; Terminales tubulares; Cinta aisladora; Termocontraible; Cintillos</t>
@@ -338,7 +338,7 @@
     <t>CAMBIO DE IRRADIADOR DE CALOR DE A.A TIPO SPLIT DE 24.000 BTU..., SPRINGER, MIDAS, CONSUL, CARRIER, JAM, JAMES, CONFORT, STAR.</t>
   </si>
   <si>
-    <t>Bomba de vacio; Cortatubos; Manifold de manometros; Soplete; Abocardador</t>
+    <t>Bomba de vacio; Cortatubos; Manifold de manómetros; Soplete; Abocardador</t>
   </si>
   <si>
     <t>Evaporador/Condensador (segun equipo); Tuberia de cobre; Aislacion termica; Filtro secador; Refrigerante (segun tipo); Cinta teflon</t>
@@ -365,7 +365,7 @@
     <t>CAMBIO DE LLAVE SELECTORA DE A.A TIPO SPLIT DE 24.000 BTU MAR..., SPRINGER, MIDAS, CONSUL, CARRIER, JAM, JAMES, CONFORT, STAR.</t>
   </si>
   <si>
-    <t>Destornilladores; Multimetro; Herramientas de mano</t>
+    <t>Destornilladores; Multímetro; Herramientas de mano</t>
   </si>
   <si>
     <t>Llave selectora/selector (segun equipo); Terminales faston; Cinta aisladora; Termocontraible; Cintillos</t>
@@ -377,7 +377,7 @@
     <t>CAMBIO DE SOLENOIDE DE A.A TIPO SPLIT DE 24.000 BTU MARCA: RB..., SPRINGER, MIDAS, CONSUL, CARRIER, JAM, JAMES, CONFORT, STAR.</t>
   </si>
   <si>
-    <t>Destornilladores; Multimetro; Llave ajustable; Herramientas de mano</t>
+    <t>Destornilladores; Multímetro; Llave ajustable; Herramientas de mano</t>
   </si>
   <si>
     <t>Bobina solenoide/valvula (segun equipo); Cinta teflon; Sellador de roscas; Terminales tubulares; Cinta aisladora</t>
@@ -395,7 +395,7 @@
     <t>CAMBIO DE VÁLVULA INVERSORA DE A.A TIPO SPLIT DE 24.000 BTU M..., SPRINGER, MIDAS, CONSUL, CARRIER, JAM, JAMES, CONFORT, STAR.</t>
   </si>
   <si>
-    <t>Manifold de manometros; Bomba de vacio; Cortatubos; Soplete; Detector de fugas</t>
+    <t>Manifold de manómetros; Bomba de vacio; Cortatubos; Soplete; Detector de fugas</t>
   </si>
   <si>
     <t>Valvula inversora (4 vias); Varilla de soldadura; Nitrogeno; Refrigerante; Filtro secador; Cinta teflon</t>
@@ -422,7 +422,7 @@
     <t>Mantenimiento / Reparacion de aire acondicionado</t>
   </si>
   <si>
-    <t>Herramientas de mano; Multimetro; Manifold de manometros (si aplica)</t>
+    <t>Herramientas de mano; Multímetro; Manifold de manómetros (si aplica)</t>
   </si>
   <si>
     <t>Consumibles varios; Cinta aisladora; Cintillos; Terminales tubulares; Estaño; Flux; Refrigerante (si aplica)</t>
@@ -533,7 +533,7 @@
     <t>MONTAJE/DESMONTAJE E INSTALACIÓN DE SISTEMA DE AA TIPO SPLIT DE 12000 BTU</t>
   </si>
   <si>
-    <t>Taladro; Nivel; Llaves; Destornilladores; Manifold de manometros; Bomba de vacio; Cortatubos; Abocardador</t>
+    <t>Taladro; Nivel; Llaves; Destornilladores; Manifold de manómetros; Bomba de vacio; Cortatubos; Abocardador</t>
   </si>
   <si>
     <t>Soportes metalicos; Tacos y tornillos; Tuberia de cobre; Aislacion termica; Cinta teflon; Cable electrico; Cintillos; Canaleta (si aplica); Refrigerante (si aplica)</t>
@@ -773,7 +773,7 @@
     <t>CARGA DE GAS REFRIGERANTE POR LITRO PARA A.A TIPO CHILLER MARCA: TRANE, YORK, CARRIER, LG, SAMSUNG, MIDEA, HITACHI, DAIKIN</t>
   </si>
   <si>
-    <t>Manifold de alta/baja; Bomba de vacio; Balanza de refrigerante; Detector de fugas; Llaves de servicio; Termometro pinza</t>
+    <t>Manifold de alta/baja; Bomba de vacio; Balanza de refrigerante; Detector de fugas; Llaves de servicio; Termómetro pinza</t>
   </si>
   <si>
     <t>Refrigerante (segun chiller); Valvulas Schrader; Cinta teflon; Sellador de roscas; Aceite refrigerante (si aplica)</t>
@@ -782,7 +782,7 @@
     <t>SOLDADURA POR PERDIDA DE GAS A.A TIPO CHILLER MARCA: TRANE, YORK, CARRIER, LG, SAMSUNG, MIDEA, HITACHI, DAIKIN</t>
   </si>
   <si>
-    <t>Cortatubos; Soplete (oxi/MAP); Regulador y manometro de nitrogeno; Manifold; Detector de fugas; Abocardador</t>
+    <t>Cortatubos; Soplete (oxi/MAP); Regulador y manómetro de nitrogeno; Manifold; Detector de fugas; Abocardador</t>
   </si>
   <si>
     <t>Varilla de soldadura (plata); Nitrogeno; Refrigerante; Filtro secador; Pasta decapante; Lija/emery; Cinta teflon</t>
@@ -803,7 +803,7 @@
     <t>CAMBIO DE BOMBA DE CIRCULACION A.A TIPO CHILLER MARCA: TRANE, YORK, CARRIER, LG, SAMSUNG, MIDEA, HITACHI, DAIKIN</t>
   </si>
   <si>
-    <t>Llaves; Extractor; Multimetro; Herramientas de mano</t>
+    <t>Llaves; Extractor; Multímetro; Herramientas de mano</t>
   </si>
   <si>
     <t>Bomba de circulacion (segun caudal); Bridas; Juntas; Tornillos; Sellador de roscas; Cinta teflon</t>
@@ -830,7 +830,7 @@
     <t>MANTENIMIENTO PREVENTIVO DE A.A TIPO CHILLER</t>
   </si>
   <si>
-    <t>Herramientas de mano; Multimetro; Manifold (si aplica)</t>
+    <t>Herramientas de mano; Multímetro; Manifold (si aplica)</t>
   </si>
   <si>
     <t>Consumibles varios; Cinta aisladora; Cintillos; Terminales tubulares; Estaño; Flux; Refrigerante (si aplica); Aceite (si aplica)</t>
@@ -866,7 +866,7 @@
     <t>CARGA DE GAS REFRIGERANTE POR LITRO PARA CÁMARA FRIGORÍFICA</t>
   </si>
   <si>
-    <t>Manifold de manometros; Bomba de vacio; Balanza de refrigerante; Detector de fugas; Llaves de servicio; Termometro pinza</t>
+    <t>Manifold de manómetros; Bomba de vacio; Balanza de refrigerante; Detector de fugas; Llaves de servicio; Termómetro pinza</t>
   </si>
   <si>
     <t>Refrigerante (segun sistema); Valvulas Schrader; Nucleos Schrader; Cinta teflon; Sellador de roscas; Aceite refrigerante (si aplica)</t>
@@ -893,7 +893,7 @@
     <t>CAMBIO DE COMPRESOR EN CÁMARA FRIGORÍFICA</t>
   </si>
   <si>
-    <t>Bomba de vacio; Cortatubos; Manifold; Soplete; Multimetro</t>
+    <t>Bomba de vacio; Cortatubos; Manifold; Soplete; Multímetro</t>
   </si>
   <si>
     <t>Compresor (segun capacidad); Aceite de compresor; Filtro secador; Refrigerante; Cinta teflon; Terminales tubulares</t>
@@ -917,7 +917,7 @@
     <t>CAMBIO DE VALVULA DE EXPANSION EN CÁMARA FRIGORÍFICA</t>
   </si>
   <si>
-    <t>Llave ajustable; Manifold; Multimetro; Herramientas de mano</t>
+    <t>Llave ajustable; Manifold; Multímetro; Herramientas de mano</t>
   </si>
   <si>
     <t>Valvula de expansion (TXV/EEV); Juntas; Cinta teflon; Sellador de roscas</t>
@@ -1016,7 +1016,7 @@
     <t>MANTENIMIENTO PREVENTIVO DE VITRINA REFRIGERADA</t>
   </si>
   <si>
-    <t>Herramientas de mano; Multimetro</t>
+    <t>Herramientas de mano; Multímetro</t>
   </si>
   <si>
     <t>Consumibles varios; Desinfectante; Cinta aisladora; Cintillos</t>
@@ -1121,7 +1121,7 @@
     <t>DIAGNÓSTICO TÉCNICO DE EQUIPOS DE REFRIGERACIÓN</t>
   </si>
   <si>
-    <t>Herramientas de mano; Multimetro; Manifold; Termometro pinza</t>
+    <t>Herramientas de mano; Multímetro; Manifold; Termómetro pinza</t>
   </si>
   <si>
     <t>Consumibles varios; Cinta aisladora; Terminales; Cintillos</t>
@@ -1130,7 +1130,7 @@
     <t>SERVICIO TÉCNICO DE EMERGENCIA EN REFRIGERACIÓN</t>
   </si>
   <si>
-    <t>Herramientas de mano; Multimetro; Manifold; Detector de fugas</t>
+    <t>Herramientas de mano; Multímetro; Manifold; Detector de fugas</t>
   </si>
   <si>
     <t>Consumibles varios; Refrigerante; Terminales; Cinta aisladora; Cintillos</t>
@@ -1154,7 +1154,7 @@
     <t>ARREGLO DE CABLEADO EN A.A TIPO PORTATIL</t>
   </si>
   <si>
-    <t>Herramientas de mano; Multimetro; Pelacables; Crimpadora</t>
+    <t>Herramientas de mano; Multímetro; Pelacables; Crimpadora</t>
   </si>
   <si>
     <t>LIMPIEZA Y MANTENIMIENTO DE A.A TIPO PORTATIL</t>
@@ -1220,7 +1220,7 @@
     <t>PRUEBA DE HERMETICIDAD CON NITRÓGENO</t>
   </si>
   <si>
-    <t>Regulador de nitrogeno; Manometro; Mangueras; Detector de fugas</t>
+    <t>Regulador de nitrogeno; manómetro; Mangueras; Detector de fugas</t>
   </si>
   <si>
     <t>Nitrogeno; Tapones; Cinta teflon; Sellador</t>
@@ -1229,7 +1229,7 @@
     <t>VACÍO PROFUNDO DEL SISTEMA</t>
   </si>
   <si>
-    <t>Bomba de vacio; Vacuometro; Mangueras</t>
+    <t>Bomba de vacio; Vacuómetro; Mangueras</t>
   </si>
   <si>
     <t>Aceite para bomba; Juntas; Tapones</t>
@@ -1238,13 +1238,13 @@
     <t>PUESTA EN MARCHA Y AJUSTES FINALES</t>
   </si>
   <si>
-    <t>Herramientas de mano; Multimetro; Termometro pinza</t>
+    <t>Herramientas de mano; Multímetro; Termómetro pinza</t>
   </si>
   <si>
     <t>MANTENIMIENTO DE A.A TIPO WINDOW / VENTANA</t>
   </si>
   <si>
-    <t>Herramientas de mano; Multimetro; Cepillos; Aspiradora/sopladora</t>
+    <t>Herramientas de mano; Multímetro; Cepillos; Aspiradora/sopladora</t>
   </si>
   <si>
     <t>Limpiador; Desinfectante; Trapos; Cinta de enmascarar; Cintillos</t>
@@ -1316,7 +1316,7 @@
     <t>SERVICIO DE AJUSTE DE CARGA Y OPTIMIZACIÓN DEL SISTEMA</t>
   </si>
   <si>
-    <t>Manifold; Multimetro; Termometro pinza</t>
+    <t>Manifold; Multímetro; Termómetro pinza</t>
   </si>
   <si>
     <t>Refrigerante; Cinta teflon; Sellador; Consumibles varios</t>
@@ -1424,7 +1424,7 @@
     <t>SERVICIO DE ASISTENCIA TÉCNICA GENERAL EN REFRIGERACIÓN</t>
   </si>
   <si>
-    <t>Herramientas de mano; Multimetro; Manifold</t>
+    <t>Herramientas de mano; Multímetro; Manifold</t>
   </si>
   <si>
     <t>Consumibles varios; Terminales; Estaño; Flux; Cinta aisladora; Cintillos</t>
@@ -1487,7 +1487,7 @@
     <t>CAMBIO DE BOMBA DE CIRCULACIÓN EN ENFRIADOR DE AGUA INDUSTRIAL</t>
   </si>
   <si>
-    <t>Llaves; Multimetro; Herramientas de mano</t>
+    <t>Llaves; Multímetro; Herramientas de mano</t>
   </si>
   <si>
     <t>Bomba de circulacion; Bridas; Juntas; Tornilleria; Sellador de roscas</t>
@@ -1625,7 +1625,7 @@
     <t>CAMBIO DE VENTILADOR / TURBINA EN A.A CENTRAL</t>
   </si>
   <si>
-    <t>Herramientas de mano; Multimetro; Pinza amperimetrica</t>
+    <t>Herramientas de mano; Multímetro; Pinza amperimétrica</t>
   </si>
   <si>
     <t>Motor ventilador; Turbina; Capacitor; Terminales; Cinta aisladora; Cintillos</t>
@@ -1898,7 +1898,7 @@
     <t>INSTALACIÓN DE ALIMENTACIÓN ELÉCTRICA MONOFÁSICA PARA EQUIPO DE A.A</t>
   </si>
   <si>
-    <t>Herramientas de mano; Multimetro; Pelacables; Crimpadora; Taladro</t>
+    <t>Herramientas de mano; Multímetro; Pelacables; Crimpadora; Taladro</t>
   </si>
   <si>
     <t>Cable de cobre; Terminales tubulares; Terminales horquilla; Cinta aisladora; Termocontraible; Cintillos; Caño corrugado</t>
@@ -1907,7 +1907,7 @@
     <t>INSTALACIÓN DE ALIMENTACIÓN ELÉCTRICA TRIFÁSICA PARA EQUIPO DE A.A</t>
   </si>
   <si>
-    <t>Herramientas de mano; Multimetro; Pinza amperimetrica; Pelacables; Crimpadora</t>
+    <t>Herramientas de mano; Multímetro; Pinza amperimétrica; Pelacables; Crimpadora</t>
   </si>
   <si>
     <t>Cable de cobre trifasico; Terminales tubulares; Terminales horquilla; Cinta aisladora; Termocontraible; Cintillos; Caño corrugado</t>
@@ -1943,7 +1943,7 @@
     <t>CONEXIÓN ELÉCTRICA DE EQUIPO DE A.A</t>
   </si>
   <si>
-    <t>Herramientas de mano; Multimetro; Destornilladores</t>
+    <t>Herramientas de mano; Multímetro; Destornilladores</t>
   </si>
   <si>
     <t>Terminales tubulares; Terminales horquilla; Cinta aisladora; Termocontraible; Cintillos</t>
@@ -2054,7 +2054,7 @@
     <t>ARMADO DE TABLERO ELÉCTRICO</t>
   </si>
   <si>
-    <t>Herramientas de mano; Destornilladores; Multimetro</t>
+    <t>Herramientas de mano; Destornilladores; Multímetro</t>
   </si>
   <si>
     <t>Termomagneticos; Diferenciales; Borneras; Contactores; Rele termico; Cableado; Etiquetas</t>
@@ -2459,7 +2459,7 @@
     <t>PRUEBA DE VACÍO FINAL DEL SISTEMA</t>
   </si>
   <si>
-    <t>Bomba de vacio; Vacuometro</t>
+    <t>Bomba de vacio; Vacuómetro</t>
   </si>
   <si>
     <t>Aceite para bomba; Juntas; Etiquetas</t>
@@ -2513,6 +2513,9 @@
     <t>ENTREGA DE MANUALES Y DOCUMENTACIÓN</t>
   </si>
   <si>
+    <t>Bolígrafo; Presilladora; Perforadora; Computadora; Tablet</t>
+  </si>
+  <si>
     <t>Manuales impresos; Carpetas; Etiquetas</t>
   </si>
   <si>
@@ -2525,6 +2528,9 @@
     <t>LIMPIEZA FINAL DE OBRA</t>
   </si>
   <si>
+    <t>Escoba, repasador, aspiradora</t>
+  </si>
+  <si>
     <t>Productos de limpieza; Bolsas; Trapos</t>
   </si>
   <si>
@@ -2558,7 +2564,360 @@
     <t>Acta definitiva; Documentación final</t>
   </si>
   <si>
+    <t>Demolicion de contrapiso y piso con aislacion existente. Incluye retiro de escombro</t>
+  </si>
+  <si>
+    <t>Carretilla; Palas; Nivel/cinta métrica; EPP básico (guantes, lentes, casco)</t>
+  </si>
+  <si>
+    <t>Flete/retiro de escombros; Cinta de señalización; Plástico protector</t>
+  </si>
+  <si>
+    <t>Provision de carpeta</t>
+  </si>
+  <si>
+    <t>Mezcladora/hormigonera; Regla de aluminio; Llana/fratacho; EPP básico (guantes, lentes, casco)</t>
+  </si>
+  <si>
+    <t>Film/polietileno; Cemento; Arena</t>
+  </si>
+  <si>
+    <t>Mano de obra de carpeta</t>
+  </si>
+  <si>
+    <t>Consumibles menores</t>
+  </si>
+  <si>
+    <t>Provision de membrana liquida y tela bidim para aislacion de losa</t>
+  </si>
+  <si>
+    <t>Taladro con hélice mezcladora; Cutter/tijera; Cepillos/hidrolavadora; EPP básico (guantes, lentes, casco)</t>
+  </si>
+  <si>
+    <t>Imprimante/sellador; Membrana líquida impermeabilizante; Tela bidim (geotextil)</t>
+  </si>
+  <si>
+    <t>Mano de obra de membrana liquida y tela bidim para aislacion de losa</t>
+  </si>
+  <si>
+    <t>Cinta de refuerzo; Consumibles menores</t>
+  </si>
+  <si>
+    <t>Remocion de revoque en zonas deterioradas</t>
+  </si>
+  <si>
+    <t>Amoladora; Barreta/cincel; Carretilla; EPP básico (guantes, lentes, casco)</t>
+  </si>
+  <si>
+    <t>Provision de revoque interior con hidrofugo</t>
+  </si>
+  <si>
+    <t>Llana/fratacho; Balde mezclador; Regla; EPP básico (guantes, lentes, casco)</t>
+  </si>
+  <si>
+    <t>Aditivo hidrófugo; Malla de fibra (si fisuras); Cemento</t>
+  </si>
+  <si>
+    <t>Mano de obra - Revoque con hidrófugo</t>
+  </si>
+  <si>
+    <t>Andamio/escalera; Llana/fratacho; Balde mezclador; EPP básico (guantes, lentes, casco)</t>
+  </si>
+  <si>
+    <t>EPP básico</t>
+  </si>
+  <si>
+    <t>Provision de pintura latex para interior con enduido</t>
+  </si>
+  <si>
+    <t>Lijas; Cinta de enmascarar; Escalera; EPP básico (guantes, lentes, casco)</t>
+  </si>
+  <si>
+    <t>Lijas; Pintura látex (interior/exterior); Enduido</t>
+  </si>
+  <si>
+    <t>Mano de obra de pintura latex para interior con enduido</t>
+  </si>
+  <si>
+    <t>Bandeja; Espátula; Lijas; EPP básico (guantes, lentes, casco)</t>
+  </si>
+  <si>
+    <t>Cinta de enmascarar; Consumibles menores</t>
+  </si>
+  <si>
+    <t>Mantenimiento de canaleta embutida  bajada</t>
+  </si>
+  <si>
+    <t>Taladro; Nivel/plomada; Amoladora; EPP básico (guantes, lentes, casco)</t>
+  </si>
+  <si>
+    <t>Tornillería y tarugos; Canaleta/bajante (según especificación); Abrazaderas/soportes</t>
+  </si>
+  <si>
+    <t>Remocion de canaleta embutida  bajada</t>
+  </si>
+  <si>
+    <t>Palas; Nivel/cinta métrica; Martillo demoledor/rotomartillo; EPP básico (guantes, lentes, casco)</t>
+  </si>
+  <si>
+    <t>Bolsas para escombro; Flete/retiro de escombros; Cinta de señalización</t>
+  </si>
+  <si>
+    <t>Provision de Canaleta embutida  bajada</t>
+  </si>
+  <si>
+    <t>Nivel/plomada; Amoladora; Rotomartillo; EPP básico (guantes, lentes, casco)</t>
+  </si>
+  <si>
+    <t>Canaleta/bajante (según especificación); Abrazaderas/soportes; Sellador (PU/silicona)</t>
+  </si>
+  <si>
+    <t>Mano de obra - instalaci撑 de Canaleta embutida + bajada</t>
+  </si>
+  <si>
+    <t>Rotomartillo; Pistola de sellador; Taladro; EPP básico (guantes, lentes, casco)</t>
+  </si>
+  <si>
+    <t>Consumibles menores; Sellador</t>
+  </si>
+  <si>
+    <t>Mantenimiento de registro pluviales</t>
+  </si>
+  <si>
+    <t>Abrazaderas/soportes; Sellador (PU/silicona); Tornillería y tarugos</t>
+  </si>
+  <si>
+    <t>Remocion de revoque en zona de humedad</t>
+  </si>
+  <si>
+    <t>Plástico protector; Bolsas para escombro; Flete/retiro de escombros</t>
+  </si>
+  <si>
+    <t>Provision de pintura latex para exterior</t>
+  </si>
+  <si>
+    <t>Pintura látex (interior/exterior); Enduido; Sellador/fijador</t>
+  </si>
+  <si>
+    <t>Mano de obra de  pintura latex para exterior</t>
+  </si>
+  <si>
+    <t>Cinta de enmascarar; Escalera; Rodillo/brocha; EPP básico (guantes, lentes, casco)</t>
+  </si>
+  <si>
+    <t>Consumibles menores; Cinta de enmascarar</t>
+  </si>
+  <si>
+    <t>Restauracion y pintura de porton corredizo existente</t>
+  </si>
+  <si>
+    <t>Masilla; Lijas; Primer/antióxido (si metal)</t>
+  </si>
+  <si>
+    <t>Bandeja de montaje de instalacion con tapa de 50 cm de ancho x 8 cm de alto. Incluye accesorios para montaje e instalacion.</t>
+  </si>
+  <si>
+    <t>Cizalla/amoladora (corte bandeja); Taladro percutor; Atornillador; EPP básico (guantes, lentes, casco)</t>
+  </si>
+  <si>
+    <t>Uniones/conectores; Bandeja portacables; Tapa de bandeja</t>
+  </si>
+  <si>
+    <t>Bandeja de 5 cm de ancho con accesorios de montaje e instalacion</t>
+  </si>
+  <si>
+    <t>Conductor nyy 4x2 mm2</t>
+  </si>
+  <si>
+    <t>Crimpeadora; Guía pasacables; Multímetro; EPP básico (guantes, lentes, casco)</t>
+  </si>
+  <si>
+    <t>Termocontraíble; Cinta aislante; Cintillos/grampas</t>
+  </si>
+  <si>
+    <t>Llave externa de un punto</t>
+  </si>
+  <si>
+    <t>Probador de tensión; Taladro; Pinza universal; EPP básico (guantes, lentes, casco)</t>
+  </si>
+  <si>
+    <t>Caja/tapa (si aplica); Conectores (regleta/Wago); Tornillería</t>
+  </si>
+  <si>
+    <t>Toma tipo nema - toma schuko</t>
+  </si>
+  <si>
+    <t>Taladro; Destornilladores aislados; Probador de tensión; EPP básico (guantes, lentes, casco)</t>
+  </si>
+  <si>
+    <t>Tornillería; Toma NEMA/Schuko; Caja para toma</t>
+  </si>
+  <si>
+    <t>Mano de obra para instalacion para puntos y tomas</t>
+  </si>
+  <si>
+    <t>Herramientas de mano; EPP básico</t>
+  </si>
+  <si>
+    <t>Adecuacion de cañerias y cables de instalacion electrica existente</t>
+  </si>
+  <si>
+    <t>Pelacables; Cortacables; Crimpeadora; EPP básico (guantes, lentes, casco)</t>
+  </si>
+  <si>
+    <t>Cable NYY 4x2 mm²; Terminales; Termocontraíble</t>
+  </si>
+  <si>
+    <t>Provisi撑 y colocaci撑 de Tablero seccionel plastico</t>
+  </si>
+  <si>
+    <t>Prensa terminales; Taladro; Destornilladores aislados; EPP básico (guantes, lentes, casco)</t>
+  </si>
+  <si>
+    <t>Terminales; Peine/busbar (si aplica); Tablero (riel DIN)</t>
+  </si>
+  <si>
+    <t>Proveer e instalar disyuntor
+Termomatnético tripolar de 80A hasta
+100A (llave dentro deltablero)</t>
+  </si>
+  <si>
+    <t>Pinza amperimétrica; Multímetro; Prensa terminales; EPP básico (guantes, lentes, casco)</t>
+  </si>
+  <si>
+    <t>Borneras; Etiquetas; Terminales</t>
+  </si>
+  <si>
+    <t>Provisi撑 de Mamparas de  tabique tipo eucatex blanco mas vidrio 50%.</t>
+  </si>
+  <si>
+    <t>Nivel; Sierra caladora; Escuadra/cinta métrica; EPP básico (guantes, lentes, casco)</t>
+  </si>
+  <si>
+    <t>Tornillería/tarugos; Placas eucatex blanco; Perfilería</t>
+  </si>
+  <si>
+    <t>Mano de Obra - Instalacion de mamparas de tabique tipo eucatex blanco mas vidrio 50%.</t>
+  </si>
+  <si>
+    <t>Taladro/atornillador; Nivel; Sierra caladora; EPP básico (guantes, lentes, casco)</t>
+  </si>
+  <si>
+    <t>Consumibles menores; Silicona neutra</t>
+  </si>
+  <si>
+    <t>Demalicion sin recuperacion de mamposteria</t>
+  </si>
+  <si>
+    <t>Nivel/cinta métrica; Martillo demoledor/rotomartillo; Amoladora; EPP básico (guantes, lentes, casco)</t>
+  </si>
+  <si>
+    <t>Dintel sobre abertura</t>
+  </si>
+  <si>
+    <t>Amoladora; Cinta métrica; Nivel; EPP básico (guantes, lentes, casco)</t>
+  </si>
+  <si>
+    <t>Cemento y arena; Encofrado (madera); Alambre de atar</t>
+  </si>
+  <si>
+    <t>Mano de obra de Dintel sobre abertura</t>
+  </si>
+  <si>
+    <t>Cinta métrica; Nivel; Mezcladora/balde; EPP básico (guantes, lentes, casco)</t>
+  </si>
+  <si>
+    <t>Provisi撑 Marco de Madera para puerta tipo placa de 0.80x2.10 m, incluye accesorios</t>
+  </si>
+  <si>
+    <t>Espuma expansiva (aplicación); Taladro; Nivel/plomada; EPP básico (guantes, lentes, casco)</t>
+  </si>
+  <si>
+    <t>Tornillería; Espuma PU/sellador; Marco/puerta (según ítem)</t>
+  </si>
+  <si>
+    <t>Instalacion de Marco de Madera para puerta tipo placa de 0.80x2.10 m, incluye accesorios</t>
+  </si>
+  <si>
+    <t>Taladro; Nivel/plomada; Atornillador; EPP básico (guantes, lentes, casco)</t>
+  </si>
+  <si>
+    <t>Espuma PU/sellador; Marco/puerta (según ítem); Bisagras</t>
+  </si>
+  <si>
+    <t>Provisi撑 Puerta de Madera tipo placa de 0.80x2.10 m, incluye accesorios</t>
+  </si>
+  <si>
+    <t>Nivel/plomada; Atornillador; Espuma expansiva (aplicación); EPP básico (guantes, lentes, casco)</t>
+  </si>
+  <si>
+    <t>Instalacion de Puerta de Madera tipo placa de 0.80x2.10 m, incluye accesorios</t>
+  </si>
+  <si>
+    <t>Marco/puerta (según ítem); Bisagras; Cerradura/manija</t>
+  </si>
+  <si>
+    <t>Provision de pintura para aberturas</t>
+  </si>
+  <si>
+    <t>Mano de obra de pintura para aberturas</t>
+  </si>
+  <si>
+    <t>Espátula; Lijas; Cinta de enmascarar; EPP básico (guantes, lentes, casco)</t>
+  </si>
+  <si>
+    <t>Provision de Ventana de Blindex  1 x  1 con sus accesorios</t>
+  </si>
+  <si>
+    <t>Nivel; Ventosas/guantes para vidrio; Pistola de silicona; EPP básico (guantes, lentes, casco)</t>
+  </si>
+  <si>
+    <t>Vidrio Blindex/templado; Silicona neutra; Tornillería/tarugos</t>
+  </si>
+  <si>
+    <t>Provision de materiales para cielorraso tecnico desmontable en placas de yeso de 60x60 con estructura de aluminio</t>
+  </si>
+  <si>
+    <t>Nivel láser; Taladro percutor; Atornillador; EPP básico (guantes, lentes, casco)</t>
+  </si>
+  <si>
+    <t>Placas 60x60; Perfilería aluminio; Colgantes/varillas</t>
+  </si>
+  <si>
+    <t>Mano de obra de instalacion de cielorraso tecnico desmontable en placas de yeso de 60x60 con estructura de aluminio</t>
+  </si>
+  <si>
+    <t>Consumibles menores; Tornillería</t>
+  </si>
+  <si>
+    <t>Llave de un punto</t>
+  </si>
+  <si>
+    <t>Destornilladores aislados; Probador de tensión; Taladro; EPP básico (guantes, lentes, casco)</t>
+  </si>
+  <si>
+    <t>Llave/interruptor 1 punto; Caja/tapa (si aplica); Conectores (regleta/Wago)</t>
+  </si>
+  <si>
+    <t>Provision de panel de adosar de 40w - 60x60 cm , luz blanca.</t>
+  </si>
+  <si>
+    <t>Atornillador; Escalera; Destornilladores aislados; EPP básico (guantes, lentes, casco)</t>
+  </si>
+  <si>
+    <t>Conectores; Cable (si extensión); Tornillería/taquetes</t>
+  </si>
+  <si>
+    <t>Mano de obra de instalacion de panel de adosar de 40w - 60x60 cm , luz blanca.</t>
+  </si>
+  <si>
+    <t>Cinta aislante; Consumibles menores</t>
+  </si>
+  <si>
     <t>DEFAULT</t>
+  </si>
+  <si>
+    <t>Herramientas de mano; Caja de herramientas</t>
   </si>
   <si>
     <t>Insumos y materiales</t>
@@ -2574,7 +2933,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2584,6 +2943,13 @@
     </font>
     <font>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <charset val="134"/>
@@ -3044,31 +3410,28 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3077,123 +3440,127 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3669,10 +4036,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C981"/>
+  <dimension ref="A1:C1026"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A476" workbookViewId="0">
-      <selection activeCell="A506" sqref="A506"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6285714285714" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="2"/>
@@ -9154,324 +9521,594 @@
         <v>826</v>
       </c>
       <c r="B498" s="1" t="s">
-        <v>7</v>
+        <v>827</v>
       </c>
       <c r="C498" s="1" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
     </row>
     <row r="499" customHeight="1" spans="1:3">
       <c r="A499" s="1" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="B499" s="1" t="s">
-        <v>7</v>
+        <v>827</v>
       </c>
       <c r="C499" s="1" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
     </row>
     <row r="500" customHeight="1" spans="1:3">
       <c r="A500" s="1" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="B500" s="1" t="s">
-        <v>7</v>
+        <v>832</v>
       </c>
       <c r="C500" s="1" t="s">
-        <v>831</v>
+        <v>833</v>
       </c>
     </row>
     <row r="501" customHeight="1" spans="1:3">
       <c r="A501" s="1" t="s">
-        <v>832</v>
+        <v>834</v>
       </c>
       <c r="B501" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C501" s="1" t="s">
-        <v>833</v>
+        <v>835</v>
       </c>
     </row>
     <row r="502" customHeight="1" spans="1:3">
       <c r="A502" s="1" t="s">
-        <v>834</v>
+        <v>836</v>
       </c>
       <c r="B502" s="1" t="s">
-        <v>7</v>
+        <v>827</v>
       </c>
       <c r="C502" s="1" t="s">
-        <v>835</v>
+        <v>837</v>
       </c>
     </row>
     <row r="503" customHeight="1" spans="1:3">
       <c r="A503" s="1" t="s">
-        <v>836</v>
+        <v>838</v>
       </c>
       <c r="B503" s="1" t="s">
-        <v>7</v>
+        <v>827</v>
       </c>
       <c r="C503" s="1" t="s">
-        <v>837</v>
+        <v>839</v>
       </c>
     </row>
     <row r="504" customHeight="1" spans="1:3">
       <c r="A504" s="1" t="s">
-        <v>838</v>
+        <v>840</v>
       </c>
       <c r="B504" s="1" t="s">
-        <v>7</v>
+        <v>827</v>
       </c>
       <c r="C504" s="1" t="s">
-        <v>839</v>
+        <v>841</v>
       </c>
     </row>
     <row r="505" customHeight="1" spans="1:3">
       <c r="A505" s="1" t="s">
-        <v>840</v>
+        <v>842</v>
       </c>
       <c r="B505" s="1" t="s">
-        <v>7</v>
+        <v>827</v>
       </c>
       <c r="C505" s="1" t="s">
-        <v>841</v>
+        <v>843</v>
       </c>
     </row>
     <row r="506" customHeight="1" spans="1:3">
-      <c r="A506" s="1" t="s">
-        <v>842</v>
-      </c>
-      <c r="B506" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C506" s="1" t="s">
-        <v>843</v>
+      <c r="A506" s="2" t="s">
+        <v>844</v>
+      </c>
+      <c r="B506" s="2" t="s">
+        <v>845</v>
+      </c>
+      <c r="C506" s="2" t="s">
+        <v>846</v>
       </c>
     </row>
     <row r="507" customHeight="1" spans="1:3">
-      <c r="A507" s="1"/>
-      <c r="B507" s="1"/>
-      <c r="C507" s="1"/>
+      <c r="A507" s="2" t="s">
+        <v>847</v>
+      </c>
+      <c r="B507" s="2" t="s">
+        <v>848</v>
+      </c>
+      <c r="C507" s="2" t="s">
+        <v>849</v>
+      </c>
     </row>
     <row r="508" customHeight="1" spans="1:3">
-      <c r="A508" s="1"/>
-      <c r="B508" s="1"/>
-      <c r="C508" s="1"/>
+      <c r="A508" s="2" t="s">
+        <v>850</v>
+      </c>
+      <c r="B508" s="2" t="s">
+        <v>848</v>
+      </c>
+      <c r="C508" s="2" t="s">
+        <v>851</v>
+      </c>
     </row>
     <row r="509" customHeight="1" spans="1:3">
-      <c r="A509" s="1"/>
-      <c r="B509" s="1"/>
-      <c r="C509" s="1"/>
+      <c r="A509" s="2" t="s">
+        <v>852</v>
+      </c>
+      <c r="B509" s="2" t="s">
+        <v>853</v>
+      </c>
+      <c r="C509" s="2" t="s">
+        <v>854</v>
+      </c>
     </row>
     <row r="510" customHeight="1" spans="1:3">
-      <c r="A510" s="1"/>
-      <c r="B510" s="1"/>
-      <c r="C510" s="1"/>
+      <c r="A510" s="2" t="s">
+        <v>855</v>
+      </c>
+      <c r="B510" s="2" t="s">
+        <v>853</v>
+      </c>
+      <c r="C510" s="2" t="s">
+        <v>856</v>
+      </c>
     </row>
     <row r="511" customHeight="1" spans="1:3">
-      <c r="A511" s="1"/>
-      <c r="B511" s="1"/>
-      <c r="C511" s="1"/>
+      <c r="A511" s="2" t="s">
+        <v>857</v>
+      </c>
+      <c r="B511" s="2" t="s">
+        <v>858</v>
+      </c>
+      <c r="C511" s="2" t="s">
+        <v>846</v>
+      </c>
     </row>
     <row r="512" customHeight="1" spans="1:3">
-      <c r="A512" s="1"/>
-      <c r="B512" s="1"/>
-      <c r="C512" s="1"/>
+      <c r="A512" s="2" t="s">
+        <v>859</v>
+      </c>
+      <c r="B512" s="2" t="s">
+        <v>860</v>
+      </c>
+      <c r="C512" s="2" t="s">
+        <v>861</v>
+      </c>
     </row>
     <row r="513" customHeight="1" spans="1:3">
-      <c r="A513" s="1"/>
-      <c r="B513" s="1"/>
-      <c r="C513" s="1"/>
+      <c r="A513" s="2" t="s">
+        <v>862</v>
+      </c>
+      <c r="B513" s="2" t="s">
+        <v>863</v>
+      </c>
+      <c r="C513" s="2" t="s">
+        <v>864</v>
+      </c>
     </row>
     <row r="514" customHeight="1" spans="1:3">
-      <c r="A514" s="1"/>
-      <c r="B514" s="1"/>
-      <c r="C514" s="1"/>
+      <c r="A514" s="2" t="s">
+        <v>865</v>
+      </c>
+      <c r="B514" s="2" t="s">
+        <v>866</v>
+      </c>
+      <c r="C514" s="2" t="s">
+        <v>867</v>
+      </c>
     </row>
     <row r="515" customHeight="1" spans="1:3">
-      <c r="A515" s="1"/>
-      <c r="B515" s="1"/>
-      <c r="C515" s="1"/>
+      <c r="A515" s="2" t="s">
+        <v>868</v>
+      </c>
+      <c r="B515" s="2" t="s">
+        <v>869</v>
+      </c>
+      <c r="C515" s="2" t="s">
+        <v>870</v>
+      </c>
     </row>
     <row r="516" customHeight="1" spans="1:3">
-      <c r="A516" s="1"/>
-      <c r="B516" s="1"/>
-      <c r="C516" s="1"/>
+      <c r="A516" s="2" t="s">
+        <v>871</v>
+      </c>
+      <c r="B516" s="2" t="s">
+        <v>872</v>
+      </c>
+      <c r="C516" s="2" t="s">
+        <v>873</v>
+      </c>
     </row>
     <row r="517" customHeight="1" spans="1:3">
-      <c r="A517" s="1"/>
-      <c r="B517" s="1"/>
-      <c r="C517" s="1"/>
+      <c r="A517" s="2" t="s">
+        <v>874</v>
+      </c>
+      <c r="B517" s="2" t="s">
+        <v>875</v>
+      </c>
+      <c r="C517" s="2" t="s">
+        <v>876</v>
+      </c>
     </row>
     <row r="518" customHeight="1" spans="1:3">
-      <c r="A518" s="1"/>
-      <c r="B518" s="1"/>
-      <c r="C518" s="1"/>
+      <c r="A518" s="2" t="s">
+        <v>877</v>
+      </c>
+      <c r="B518" s="2" t="s">
+        <v>878</v>
+      </c>
+      <c r="C518" s="2" t="s">
+        <v>879</v>
+      </c>
     </row>
     <row r="519" customHeight="1" spans="1:3">
-      <c r="A519" s="1"/>
-      <c r="B519" s="1"/>
-      <c r="C519" s="1"/>
+      <c r="A519" s="2" t="s">
+        <v>880</v>
+      </c>
+      <c r="B519" s="2" t="s">
+        <v>881</v>
+      </c>
+      <c r="C519" s="2" t="s">
+        <v>882</v>
+      </c>
     </row>
     <row r="520" customHeight="1" spans="1:3">
-      <c r="A520" s="1"/>
-      <c r="B520" s="1"/>
-      <c r="C520" s="1"/>
+      <c r="A520" s="2" t="s">
+        <v>883</v>
+      </c>
+      <c r="B520" s="2" t="s">
+        <v>881</v>
+      </c>
+      <c r="C520" s="2" t="s">
+        <v>884</v>
+      </c>
     </row>
     <row r="521" customHeight="1" spans="1:3">
-      <c r="A521" s="1"/>
-      <c r="B521" s="1"/>
-      <c r="C521" s="1"/>
+      <c r="A521" s="2" t="s">
+        <v>885</v>
+      </c>
+      <c r="B521" s="2" t="s">
+        <v>845</v>
+      </c>
+      <c r="C521" s="2" t="s">
+        <v>886</v>
+      </c>
     </row>
     <row r="522" customHeight="1" spans="1:3">
-      <c r="A522" s="1"/>
-      <c r="B522" s="1"/>
-      <c r="C522" s="1"/>
+      <c r="A522" s="2" t="s">
+        <v>887</v>
+      </c>
+      <c r="B522" s="2" t="s">
+        <v>866</v>
+      </c>
+      <c r="C522" s="2" t="s">
+        <v>888</v>
+      </c>
     </row>
     <row r="523" customHeight="1" spans="1:3">
-      <c r="A523" s="1"/>
-      <c r="B523" s="1"/>
-      <c r="C523" s="1"/>
+      <c r="A523" s="2" t="s">
+        <v>889</v>
+      </c>
+      <c r="B523" s="2" t="s">
+        <v>890</v>
+      </c>
+      <c r="C523" s="2" t="s">
+        <v>891</v>
+      </c>
     </row>
     <row r="524" customHeight="1" spans="1:3">
-      <c r="A524" s="1"/>
-      <c r="B524" s="1"/>
-      <c r="C524" s="1"/>
+      <c r="A524" s="2" t="s">
+        <v>892</v>
+      </c>
+      <c r="B524" s="2" t="s">
+        <v>869</v>
+      </c>
+      <c r="C524" s="2" t="s">
+        <v>893</v>
+      </c>
     </row>
     <row r="525" customHeight="1" spans="1:3">
-      <c r="A525" s="1"/>
-      <c r="B525" s="1"/>
-      <c r="C525" s="1"/>
+      <c r="A525" s="2" t="s">
+        <v>894</v>
+      </c>
+      <c r="B525" s="2" t="s">
+        <v>895</v>
+      </c>
+      <c r="C525" s="2" t="s">
+        <v>896</v>
+      </c>
     </row>
     <row r="526" customHeight="1" spans="1:3">
-      <c r="A526" s="1"/>
-      <c r="B526" s="1"/>
-      <c r="C526" s="1"/>
+      <c r="A526" s="2" t="s">
+        <v>897</v>
+      </c>
+      <c r="B526" s="2" t="s">
+        <v>895</v>
+      </c>
+      <c r="C526" s="2" t="s">
+        <v>896</v>
+      </c>
     </row>
     <row r="527" customHeight="1" spans="1:3">
-      <c r="A527" s="1"/>
-      <c r="B527" s="1"/>
-      <c r="C527" s="1"/>
+      <c r="A527" s="2" t="s">
+        <v>898</v>
+      </c>
+      <c r="B527" s="2" t="s">
+        <v>899</v>
+      </c>
+      <c r="C527" s="2" t="s">
+        <v>900</v>
+      </c>
     </row>
     <row r="528" customHeight="1" spans="1:3">
-      <c r="A528" s="1"/>
-      <c r="B528" s="1"/>
-      <c r="C528" s="1"/>
+      <c r="A528" s="2" t="s">
+        <v>901</v>
+      </c>
+      <c r="B528" s="2" t="s">
+        <v>902</v>
+      </c>
+      <c r="C528" s="2" t="s">
+        <v>903</v>
+      </c>
     </row>
     <row r="529" customHeight="1" spans="1:3">
-      <c r="A529" s="1"/>
-      <c r="B529" s="1"/>
-      <c r="C529" s="1"/>
+      <c r="A529" s="2" t="s">
+        <v>904</v>
+      </c>
+      <c r="B529" s="2" t="s">
+        <v>905</v>
+      </c>
+      <c r="C529" s="2" t="s">
+        <v>906</v>
+      </c>
     </row>
     <row r="530" customHeight="1" spans="1:3">
-      <c r="A530" s="1"/>
-      <c r="B530" s="1"/>
-      <c r="C530" s="1"/>
+      <c r="A530" s="2" t="s">
+        <v>907</v>
+      </c>
+      <c r="B530" s="2" t="s">
+        <v>908</v>
+      </c>
+      <c r="C530" s="2" t="s">
+        <v>851</v>
+      </c>
     </row>
     <row r="531" customHeight="1" spans="1:3">
-      <c r="A531" s="1"/>
-      <c r="B531" s="1"/>
-      <c r="C531" s="1"/>
+      <c r="A531" s="2" t="s">
+        <v>909</v>
+      </c>
+      <c r="B531" s="2" t="s">
+        <v>910</v>
+      </c>
+      <c r="C531" s="2" t="s">
+        <v>911</v>
+      </c>
     </row>
     <row r="532" customHeight="1" spans="1:3">
-      <c r="A532" s="1"/>
-      <c r="B532" s="1"/>
-      <c r="C532" s="1"/>
+      <c r="A532" s="2" t="s">
+        <v>912</v>
+      </c>
+      <c r="B532" s="2" t="s">
+        <v>913</v>
+      </c>
+      <c r="C532" s="2" t="s">
+        <v>914</v>
+      </c>
     </row>
     <row r="533" customHeight="1" spans="1:3">
-      <c r="A533" s="1"/>
-      <c r="B533" s="1"/>
-      <c r="C533" s="1"/>
+      <c r="A533" s="2" t="s">
+        <v>915</v>
+      </c>
+      <c r="B533" s="2" t="s">
+        <v>916</v>
+      </c>
+      <c r="C533" s="2" t="s">
+        <v>917</v>
+      </c>
     </row>
     <row r="534" customHeight="1" spans="1:3">
-      <c r="A534" s="1"/>
-      <c r="B534" s="1"/>
-      <c r="C534" s="1"/>
+      <c r="A534" s="2" t="s">
+        <v>918</v>
+      </c>
+      <c r="B534" s="2" t="s">
+        <v>919</v>
+      </c>
+      <c r="C534" s="2" t="s">
+        <v>920</v>
+      </c>
     </row>
     <row r="535" customHeight="1" spans="1:3">
-      <c r="A535" s="1"/>
-      <c r="B535" s="1"/>
-      <c r="C535" s="1"/>
+      <c r="A535" s="2" t="s">
+        <v>921</v>
+      </c>
+      <c r="B535" s="2" t="s">
+        <v>922</v>
+      </c>
+      <c r="C535" s="2" t="s">
+        <v>923</v>
+      </c>
     </row>
     <row r="536" customHeight="1" spans="1:3">
-      <c r="A536" s="1"/>
-      <c r="B536" s="1"/>
-      <c r="C536" s="1"/>
+      <c r="A536" s="2" t="s">
+        <v>924</v>
+      </c>
+      <c r="B536" s="2" t="s">
+        <v>925</v>
+      </c>
+      <c r="C536" s="2" t="s">
+        <v>886</v>
+      </c>
     </row>
     <row r="537" customHeight="1" spans="1:3">
-      <c r="A537" s="1"/>
-      <c r="B537" s="1"/>
-      <c r="C537" s="1"/>
+      <c r="A537" s="2" t="s">
+        <v>926</v>
+      </c>
+      <c r="B537" s="2" t="s">
+        <v>927</v>
+      </c>
+      <c r="C537" s="2" t="s">
+        <v>928</v>
+      </c>
     </row>
     <row r="538" customHeight="1" spans="1:3">
-      <c r="A538" s="1"/>
-      <c r="B538" s="1"/>
-      <c r="C538" s="1"/>
+      <c r="A538" s="2" t="s">
+        <v>929</v>
+      </c>
+      <c r="B538" s="2" t="s">
+        <v>930</v>
+      </c>
+      <c r="C538" s="2" t="s">
+        <v>864</v>
+      </c>
     </row>
     <row r="539" customHeight="1" spans="1:3">
-      <c r="A539" s="1"/>
-      <c r="B539" s="1"/>
-      <c r="C539" s="1"/>
+      <c r="A539" s="2" t="s">
+        <v>931</v>
+      </c>
+      <c r="B539" s="2" t="s">
+        <v>932</v>
+      </c>
+      <c r="C539" s="2" t="s">
+        <v>933</v>
+      </c>
     </row>
     <row r="540" customHeight="1" spans="1:3">
-      <c r="A540" s="1"/>
-      <c r="B540" s="1"/>
-      <c r="C540" s="1"/>
+      <c r="A540" s="2" t="s">
+        <v>934</v>
+      </c>
+      <c r="B540" s="2" t="s">
+        <v>935</v>
+      </c>
+      <c r="C540" s="2" t="s">
+        <v>936</v>
+      </c>
     </row>
     <row r="541" customHeight="1" spans="1:3">
-      <c r="A541" s="1"/>
-      <c r="B541" s="1"/>
-      <c r="C541" s="1"/>
+      <c r="A541" s="2" t="s">
+        <v>937</v>
+      </c>
+      <c r="B541" s="2" t="s">
+        <v>938</v>
+      </c>
+      <c r="C541" s="2" t="s">
+        <v>936</v>
+      </c>
     </row>
     <row r="542" customHeight="1" spans="1:3">
-      <c r="A542" s="1"/>
-      <c r="B542" s="1"/>
-      <c r="C542" s="1"/>
+      <c r="A542" s="2" t="s">
+        <v>939</v>
+      </c>
+      <c r="B542" s="2" t="s">
+        <v>935</v>
+      </c>
+      <c r="C542" s="2" t="s">
+        <v>940</v>
+      </c>
     </row>
     <row r="543" customHeight="1" spans="1:3">
-      <c r="A543" s="1"/>
-      <c r="B543" s="1"/>
-      <c r="C543" s="1"/>
+      <c r="A543" s="2" t="s">
+        <v>941</v>
+      </c>
+      <c r="B543" s="2" t="s">
+        <v>890</v>
+      </c>
+      <c r="C543" s="2" t="s">
+        <v>893</v>
+      </c>
     </row>
     <row r="544" customHeight="1" spans="1:3">
-      <c r="A544" s="1"/>
-      <c r="B544" s="1"/>
-      <c r="C544" s="1"/>
+      <c r="A544" s="2" t="s">
+        <v>942</v>
+      </c>
+      <c r="B544" s="2" t="s">
+        <v>943</v>
+      </c>
+      <c r="C544" s="2" t="s">
+        <v>891</v>
+      </c>
     </row>
     <row r="545" customHeight="1" spans="1:3">
-      <c r="A545" s="1"/>
-      <c r="B545" s="1"/>
-      <c r="C545" s="1"/>
+      <c r="A545" s="2" t="s">
+        <v>944</v>
+      </c>
+      <c r="B545" s="2" t="s">
+        <v>945</v>
+      </c>
+      <c r="C545" s="2" t="s">
+        <v>946</v>
+      </c>
     </row>
     <row r="546" customHeight="1" spans="1:3">
-      <c r="A546" s="1"/>
-      <c r="B546" s="1"/>
-      <c r="C546" s="1"/>
+      <c r="A546" s="2" t="s">
+        <v>947</v>
+      </c>
+      <c r="B546" s="2" t="s">
+        <v>948</v>
+      </c>
+      <c r="C546" s="2" t="s">
+        <v>949</v>
+      </c>
     </row>
     <row r="547" customHeight="1" spans="1:3">
-      <c r="A547" s="1"/>
-      <c r="B547" s="1"/>
-      <c r="C547" s="1"/>
+      <c r="A547" s="2" t="s">
+        <v>950</v>
+      </c>
+      <c r="B547" s="2" t="s">
+        <v>948</v>
+      </c>
+      <c r="C547" s="2" t="s">
+        <v>951</v>
+      </c>
     </row>
     <row r="548" customHeight="1" spans="1:3">
-      <c r="A548" s="1"/>
-      <c r="B548" s="1"/>
-      <c r="C548" s="1"/>
+      <c r="A548" s="2" t="s">
+        <v>952</v>
+      </c>
+      <c r="B548" s="2" t="s">
+        <v>953</v>
+      </c>
+      <c r="C548" s="2" t="s">
+        <v>954</v>
+      </c>
     </row>
     <row r="549" customHeight="1" spans="1:3">
-      <c r="A549" s="1"/>
-      <c r="B549" s="1"/>
-      <c r="C549" s="1"/>
+      <c r="A549" s="2" t="s">
+        <v>955</v>
+      </c>
+      <c r="B549" s="2" t="s">
+        <v>956</v>
+      </c>
+      <c r="C549" s="2" t="s">
+        <v>957</v>
+      </c>
     </row>
     <row r="550" customHeight="1" spans="1:3">
-      <c r="A550" s="1"/>
-      <c r="B550" s="1"/>
-      <c r="C550" s="1"/>
+      <c r="A550" s="2" t="s">
+        <v>958</v>
+      </c>
+      <c r="B550" s="2" t="s">
+        <v>956</v>
+      </c>
+      <c r="C550" s="2" t="s">
+        <v>959</v>
+      </c>
     </row>
     <row r="551" customHeight="1" spans="1:3">
-      <c r="A551" s="1"/>
-      <c r="B551" s="1"/>
-      <c r="C551" s="1"/>
+      <c r="A551" s="1" t="s">
+        <v>960</v>
+      </c>
+      <c r="B551" s="1" t="s">
+        <v>961</v>
+      </c>
+      <c r="C551" s="1" t="s">
+        <v>962</v>
+      </c>
     </row>
     <row r="552" customHeight="1" spans="1:3">
       <c r="A552" s="1"/>
@@ -11623,8 +12260,233 @@
       <c r="B981" s="1"/>
       <c r="C981" s="1"/>
     </row>
+    <row r="982" customHeight="1" spans="1:3">
+      <c r="A982" s="1"/>
+      <c r="B982" s="1"/>
+      <c r="C982" s="1"/>
+    </row>
+    <row r="983" customHeight="1" spans="1:3">
+      <c r="A983" s="1"/>
+      <c r="B983" s="1"/>
+      <c r="C983" s="1"/>
+    </row>
+    <row r="984" customHeight="1" spans="1:3">
+      <c r="A984" s="1"/>
+      <c r="B984" s="1"/>
+      <c r="C984" s="1"/>
+    </row>
+    <row r="985" customHeight="1" spans="1:3">
+      <c r="A985" s="1"/>
+      <c r="B985" s="1"/>
+      <c r="C985" s="1"/>
+    </row>
+    <row r="986" customHeight="1" spans="1:3">
+      <c r="A986" s="1"/>
+      <c r="B986" s="1"/>
+      <c r="C986" s="1"/>
+    </row>
+    <row r="987" customHeight="1" spans="1:3">
+      <c r="A987" s="1"/>
+      <c r="B987" s="1"/>
+      <c r="C987" s="1"/>
+    </row>
+    <row r="988" customHeight="1" spans="1:3">
+      <c r="A988" s="1"/>
+      <c r="B988" s="1"/>
+      <c r="C988" s="1"/>
+    </row>
+    <row r="989" customHeight="1" spans="1:3">
+      <c r="A989" s="1"/>
+      <c r="B989" s="1"/>
+      <c r="C989" s="1"/>
+    </row>
+    <row r="990" customHeight="1" spans="1:3">
+      <c r="A990" s="1"/>
+      <c r="B990" s="1"/>
+      <c r="C990" s="1"/>
+    </row>
+    <row r="991" customHeight="1" spans="1:3">
+      <c r="A991" s="1"/>
+      <c r="B991" s="1"/>
+      <c r="C991" s="1"/>
+    </row>
+    <row r="992" customHeight="1" spans="1:3">
+      <c r="A992" s="1"/>
+      <c r="B992" s="1"/>
+      <c r="C992" s="1"/>
+    </row>
+    <row r="993" customHeight="1" spans="1:3">
+      <c r="A993" s="1"/>
+      <c r="B993" s="1"/>
+      <c r="C993" s="1"/>
+    </row>
+    <row r="994" customHeight="1" spans="1:3">
+      <c r="A994" s="1"/>
+      <c r="B994" s="1"/>
+      <c r="C994" s="1"/>
+    </row>
+    <row r="995" customHeight="1" spans="1:3">
+      <c r="A995" s="1"/>
+      <c r="B995" s="1"/>
+      <c r="C995" s="1"/>
+    </row>
+    <row r="996" customHeight="1" spans="1:3">
+      <c r="A996" s="1"/>
+      <c r="B996" s="1"/>
+      <c r="C996" s="1"/>
+    </row>
+    <row r="997" customHeight="1" spans="1:3">
+      <c r="A997" s="1"/>
+      <c r="B997" s="1"/>
+      <c r="C997" s="1"/>
+    </row>
+    <row r="998" customHeight="1" spans="1:3">
+      <c r="A998" s="1"/>
+      <c r="B998" s="1"/>
+      <c r="C998" s="1"/>
+    </row>
+    <row r="999" customHeight="1" spans="1:3">
+      <c r="A999" s="1"/>
+      <c r="B999" s="1"/>
+      <c r="C999" s="1"/>
+    </row>
+    <row r="1000" customHeight="1" spans="1:3">
+      <c r="A1000" s="1"/>
+      <c r="B1000" s="1"/>
+      <c r="C1000" s="1"/>
+    </row>
+    <row r="1001" customHeight="1" spans="1:3">
+      <c r="A1001" s="1"/>
+      <c r="B1001" s="1"/>
+      <c r="C1001" s="1"/>
+    </row>
+    <row r="1002" customHeight="1" spans="1:3">
+      <c r="A1002" s="1"/>
+      <c r="B1002" s="1"/>
+      <c r="C1002" s="1"/>
+    </row>
+    <row r="1003" customHeight="1" spans="1:3">
+      <c r="A1003" s="1"/>
+      <c r="B1003" s="1"/>
+      <c r="C1003" s="1"/>
+    </row>
+    <row r="1004" customHeight="1" spans="1:3">
+      <c r="A1004" s="1"/>
+      <c r="B1004" s="1"/>
+      <c r="C1004" s="1"/>
+    </row>
+    <row r="1005" customHeight="1" spans="1:3">
+      <c r="A1005" s="1"/>
+      <c r="B1005" s="1"/>
+      <c r="C1005" s="1"/>
+    </row>
+    <row r="1006" customHeight="1" spans="1:3">
+      <c r="A1006" s="1"/>
+      <c r="B1006" s="1"/>
+      <c r="C1006" s="1"/>
+    </row>
+    <row r="1007" customHeight="1" spans="1:3">
+      <c r="A1007" s="1"/>
+      <c r="B1007" s="1"/>
+      <c r="C1007" s="1"/>
+    </row>
+    <row r="1008" customHeight="1" spans="1:3">
+      <c r="A1008" s="1"/>
+      <c r="B1008" s="1"/>
+      <c r="C1008" s="1"/>
+    </row>
+    <row r="1009" customHeight="1" spans="1:3">
+      <c r="A1009" s="1"/>
+      <c r="B1009" s="1"/>
+      <c r="C1009" s="1"/>
+    </row>
+    <row r="1010" customHeight="1" spans="1:3">
+      <c r="A1010" s="1"/>
+      <c r="B1010" s="1"/>
+      <c r="C1010" s="1"/>
+    </row>
+    <row r="1011" customHeight="1" spans="1:3">
+      <c r="A1011" s="1"/>
+      <c r="B1011" s="1"/>
+      <c r="C1011" s="1"/>
+    </row>
+    <row r="1012" customHeight="1" spans="1:3">
+      <c r="A1012" s="1"/>
+      <c r="B1012" s="1"/>
+      <c r="C1012" s="1"/>
+    </row>
+    <row r="1013" customHeight="1" spans="1:3">
+      <c r="A1013" s="1"/>
+      <c r="B1013" s="1"/>
+      <c r="C1013" s="1"/>
+    </row>
+    <row r="1014" customHeight="1" spans="1:3">
+      <c r="A1014" s="1"/>
+      <c r="B1014" s="1"/>
+      <c r="C1014" s="1"/>
+    </row>
+    <row r="1015" customHeight="1" spans="1:3">
+      <c r="A1015" s="1"/>
+      <c r="B1015" s="1"/>
+      <c r="C1015" s="1"/>
+    </row>
+    <row r="1016" customHeight="1" spans="1:3">
+      <c r="A1016" s="1"/>
+      <c r="B1016" s="1"/>
+      <c r="C1016" s="1"/>
+    </row>
+    <row r="1017" customHeight="1" spans="1:3">
+      <c r="A1017" s="1"/>
+      <c r="B1017" s="1"/>
+      <c r="C1017" s="1"/>
+    </row>
+    <row r="1018" customHeight="1" spans="1:3">
+      <c r="A1018" s="1"/>
+      <c r="B1018" s="1"/>
+      <c r="C1018" s="1"/>
+    </row>
+    <row r="1019" customHeight="1" spans="1:3">
+      <c r="A1019" s="1"/>
+      <c r="B1019" s="1"/>
+      <c r="C1019" s="1"/>
+    </row>
+    <row r="1020" customHeight="1" spans="1:3">
+      <c r="A1020" s="1"/>
+      <c r="B1020" s="1"/>
+      <c r="C1020" s="1"/>
+    </row>
+    <row r="1021" customHeight="1" spans="1:3">
+      <c r="A1021" s="1"/>
+      <c r="B1021" s="1"/>
+      <c r="C1021" s="1"/>
+    </row>
+    <row r="1022" customHeight="1" spans="1:3">
+      <c r="A1022" s="1"/>
+      <c r="B1022" s="1"/>
+      <c r="C1022" s="1"/>
+    </row>
+    <row r="1023" customHeight="1" spans="1:3">
+      <c r="A1023" s="1"/>
+      <c r="B1023" s="1"/>
+      <c r="C1023" s="1"/>
+    </row>
+    <row r="1024" customHeight="1" spans="1:3">
+      <c r="A1024" s="1"/>
+      <c r="B1024" s="1"/>
+      <c r="C1024" s="1"/>
+    </row>
+    <row r="1025" customHeight="1" spans="1:3">
+      <c r="A1025" s="1"/>
+      <c r="B1025" s="1"/>
+      <c r="C1025" s="1"/>
+    </row>
+    <row r="1026" customHeight="1" spans="1:3">
+      <c r="A1026" s="1"/>
+      <c r="B1026" s="1"/>
+      <c r="C1026" s="1"/>
+    </row>
   </sheetData>
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:Z981" etc:filterBottomFollowUsedRange="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:Z1026" etc:filterBottomFollowUsedRange="0">
     <extLst/>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>